<commit_message>
- debugging build mode
</commit_message>
<xml_diff>
--- a/src/renderer/storage/presentations.xlsx
+++ b/src/renderer/storage/presentations.xlsx
@@ -393,13 +393,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>57b1e4a4-1c71-4c85-a66f-a6fe125cec98</v>
+        <v>9ce30980-712b-49c9-b634-43153cb94613</v>
       </c>
       <c r="B2" t="str">
-        <v>zuzuzu</v>
+        <v>eeeee eee</v>
       </c>
       <c r="C2" t="str">
-        <v>src\renderer\storage\presentation-57b1e4a4-1c71-4c85-a66f-a6fe125cec98.xlsx</v>
+        <v>src\renderer\storage\presentation-9ce30980-712b-49c9-b634-43153cb94613.xlsx</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Cleaning the code  - Build icons  - Readme update
</commit_message>
<xml_diff>
--- a/src/renderer/storage/presentations.xlsx
+++ b/src/renderer/storage/presentations.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -393,18 +393,29 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>9ce30980-712b-49c9-b634-43153cb94613</v>
+        <v>4d3c1167-0f83-461e-88a9-96df288c8e2b</v>
       </c>
       <c r="B2" t="str">
-        <v>eeeee eee</v>
+        <v>ueueuue ueueu ue</v>
       </c>
       <c r="C2" t="str">
-        <v>src\renderer\storage\presentation-9ce30980-712b-49c9-b634-43153cb94613.xlsx</v>
+        <v>src\renderer\storage\presentation-4d3c1167-0f83-461e-88a9-96df288c8e2b.xlsx</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>106f270d-ab19-49df-9e5e-eb21a141fc58</v>
+      </c>
+      <c r="B3" t="str">
+        <v>ii i ii isiad sii</v>
+      </c>
+      <c r="C3" t="str">
+        <v>src\renderer\storage\presentation-106f270d-ab19-49df-9e5e-eb21a141fc58.xlsx</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>